<commit_message>
pre war state added
</commit_message>
<xml_diff>
--- a/saves.xlsx
+++ b/saves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tblaznik\Documents\GitHub\TORN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24699C7D-2BD9-4B7D-B7B6-6E40FE6BECB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3797AFD-77B3-4F2F-B1D8-DEDADE81F590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{EA5959C1-A7FE-47AA-8A05-F6B4B1B5114A}"/>
   </bookViews>
@@ -1185,7 +1185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17E519F-1F35-4958-911A-553FE9973E19}">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1204,6 +1206,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>0</v>
       </c>
@@ -1212,6 +1217,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
       <c r="C3">
         <v>0</v>
       </c>
@@ -1220,6 +1228,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
       <c r="C4">
         <v>0</v>
       </c>
@@ -1228,6 +1239,9 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
       <c r="C5">
         <v>0</v>
       </c>
@@ -1236,6 +1250,9 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -1244,6 +1261,9 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
       <c r="C7">
         <v>0</v>
       </c>
@@ -1252,6 +1272,9 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -1260,6 +1283,9 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
       <c r="C9">
         <v>0</v>
       </c>
@@ -1268,6 +1294,9 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
       <c r="C10">
         <v>0</v>
       </c>
@@ -1277,10 +1306,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>35.58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,16 +1317,19 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>23.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
       <c r="C13">
         <v>0</v>
       </c>
@@ -1306,6 +1338,9 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
       <c r="C14">
         <v>0</v>
       </c>
@@ -1314,6 +1349,9 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
       <c r="C15">
         <v>0</v>
       </c>
@@ -1322,6 +1360,9 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
       <c r="C16">
         <v>0</v>
       </c>
@@ -1330,6 +1371,9 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
       <c r="C17">
         <v>0</v>
       </c>
@@ -1338,6 +1382,9 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
       <c r="C18">
         <v>0</v>
       </c>
@@ -1347,16 +1394,19 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>71.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
       <c r="C20">
         <v>0</v>
       </c>
@@ -1365,6 +1415,9 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
       <c r="C21">
         <v>0</v>
       </c>
@@ -1373,6 +1426,9 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
       <c r="C22">
         <v>0</v>
       </c>
@@ -1381,6 +1437,9 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
       <c r="C23">
         <v>0</v>
       </c>
@@ -1389,6 +1448,9 @@
       <c r="A24" t="s">
         <v>25</v>
       </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
       <c r="C24">
         <v>0</v>
       </c>
@@ -1397,6 +1459,9 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
       <c r="C25">
         <v>0</v>
       </c>
@@ -1405,6 +1470,9 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
       <c r="C26">
         <v>0</v>
       </c>
@@ -1413,6 +1481,9 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
       <c r="C27">
         <v>0</v>
       </c>
@@ -1422,16 +1493,19 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>11.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
       <c r="C29">
         <v>0</v>
       </c>
@@ -1440,6 +1514,9 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
       <c r="C30">
         <v>0</v>
       </c>
@@ -1448,6 +1525,9 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
       <c r="C31">
         <v>0</v>
       </c>
@@ -1456,6 +1536,9 @@
       <c r="A32" t="s">
         <v>33</v>
       </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
       <c r="C32">
         <v>0</v>
       </c>
@@ -1464,6 +1547,9 @@
       <c r="A33" t="s">
         <v>34</v>
       </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
       <c r="C33">
         <v>0</v>
       </c>
@@ -1472,6 +1558,9 @@
       <c r="A34" t="s">
         <v>35</v>
       </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
       <c r="C34">
         <v>0</v>
       </c>
@@ -1480,6 +1569,9 @@
       <c r="A35" t="s">
         <v>36</v>
       </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
       <c r="C35">
         <v>0</v>
       </c>
@@ -1488,6 +1580,9 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
       <c r="C36">
         <v>0</v>
       </c>
@@ -1496,6 +1591,9 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
       <c r="C37">
         <v>0</v>
       </c>
@@ -1504,6 +1602,9 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
       <c r="C38">
         <v>0</v>
       </c>
@@ -1512,6 +1613,9 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
       <c r="C39">
         <v>0</v>
       </c>
@@ -1520,6 +1624,9 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
       <c r="C40">
         <v>0</v>
       </c>
@@ -1528,6 +1635,9 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
       <c r="C41">
         <v>0</v>
       </c>
@@ -1536,6 +1646,9 @@
       <c r="A42" t="s">
         <v>43</v>
       </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
       <c r="C42">
         <v>0</v>
       </c>
@@ -1544,6 +1657,9 @@
       <c r="A43" t="s">
         <v>44</v>
       </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
       <c r="C43">
         <v>0</v>
       </c>
@@ -1552,6 +1668,9 @@
       <c r="A44" t="s">
         <v>45</v>
       </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
       <c r="C44">
         <v>0</v>
       </c>
@@ -1560,6 +1679,9 @@
       <c r="A45" t="s">
         <v>46</v>
       </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
       <c r="C45">
         <v>0</v>
       </c>
@@ -1568,6 +1690,9 @@
       <c r="A46" t="s">
         <v>47</v>
       </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
       <c r="C46">
         <v>0</v>
       </c>
@@ -1576,6 +1701,9 @@
       <c r="A47" t="s">
         <v>48</v>
       </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
       <c r="C47">
         <v>0</v>
       </c>
@@ -1584,6 +1712,9 @@
       <c r="A48" t="s">
         <v>49</v>
       </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
       <c r="C48">
         <v>0</v>
       </c>
@@ -1592,6 +1723,9 @@
       <c r="A49" t="s">
         <v>50</v>
       </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
       <c r="C49">
         <v>0</v>
       </c>
@@ -1600,6 +1734,9 @@
       <c r="A50" t="s">
         <v>51</v>
       </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
       <c r="C50">
         <v>0</v>
       </c>
@@ -1608,6 +1745,9 @@
       <c r="A51" t="s">
         <v>52</v>
       </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
       <c r="C51">
         <v>0</v>
       </c>
@@ -1616,6 +1756,9 @@
       <c r="A52" t="s">
         <v>53</v>
       </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
       <c r="C52">
         <v>0</v>
       </c>
@@ -1624,6 +1767,9 @@
       <c r="A53" t="s">
         <v>54</v>
       </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
       <c r="C53">
         <v>0</v>
       </c>
@@ -1632,6 +1778,9 @@
       <c r="A54" t="s">
         <v>55</v>
       </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
       <c r="C54">
         <v>0</v>
       </c>
@@ -1640,6 +1789,9 @@
       <c r="A55" t="s">
         <v>56</v>
       </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
       <c r="C55">
         <v>0</v>
       </c>
@@ -1648,6 +1800,9 @@
       <c r="A56" t="s">
         <v>57</v>
       </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
       <c r="C56">
         <v>0</v>
       </c>
@@ -1656,6 +1811,9 @@
       <c r="A57" t="s">
         <v>58</v>
       </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
       <c r="C57">
         <v>0</v>
       </c>
@@ -1664,6 +1822,9 @@
       <c r="A58" t="s">
         <v>59</v>
       </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
       <c r="C58">
         <v>0</v>
       </c>
@@ -1672,6 +1833,9 @@
       <c r="A59" t="s">
         <v>60</v>
       </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
       <c r="C59">
         <v>0</v>
       </c>
@@ -1681,10 +1845,10 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>11.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1692,16 +1856,19 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>11.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
       <c r="C62">
         <v>0</v>
       </c>
@@ -1710,6 +1877,9 @@
       <c r="A63" t="s">
         <v>64</v>
       </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
       <c r="C63">
         <v>0</v>
       </c>
@@ -1718,6 +1888,9 @@
       <c r="A64" t="s">
         <v>65</v>
       </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
       <c r="C64">
         <v>0</v>
       </c>
@@ -1726,6 +1899,9 @@
       <c r="A65" t="s">
         <v>66</v>
       </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
       <c r="C65">
         <v>0</v>
       </c>
@@ -1734,6 +1910,9 @@
       <c r="A66" t="s">
         <v>67</v>
       </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
       <c r="C66">
         <v>0</v>
       </c>
@@ -1742,6 +1921,9 @@
       <c r="A67" t="s">
         <v>68</v>
       </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
       <c r="C67">
         <v>0</v>
       </c>
@@ -1750,6 +1932,9 @@
       <c r="A68" t="s">
         <v>69</v>
       </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
       <c r="C68">
         <v>0</v>
       </c>
@@ -1758,6 +1943,9 @@
       <c r="A69" t="s">
         <v>70</v>
       </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
       <c r="C69">
         <v>0</v>
       </c>
@@ -1766,6 +1954,9 @@
       <c r="A70" t="s">
         <v>71</v>
       </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
       <c r="C70">
         <v>0</v>
       </c>
@@ -1774,6 +1965,9 @@
       <c r="A71" t="s">
         <v>72</v>
       </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
       <c r="C71">
         <v>0</v>
       </c>
@@ -1782,6 +1976,9 @@
       <c r="A72" t="s">
         <v>73</v>
       </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
       <c r="C72">
         <v>0</v>
       </c>
@@ -1790,6 +1987,9 @@
       <c r="A73" t="s">
         <v>74</v>
       </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
       <c r="C73">
         <v>0</v>
       </c>
@@ -1798,6 +1998,9 @@
       <c r="A74" t="s">
         <v>75</v>
       </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
       <c r="C74">
         <v>0</v>
       </c>
@@ -1806,6 +2009,9 @@
       <c r="A75" t="s">
         <v>76</v>
       </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
       <c r="C75">
         <v>0</v>
       </c>
@@ -1814,6 +2020,9 @@
       <c r="A76" t="s">
         <v>77</v>
       </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
       <c r="C76">
         <v>0</v>
       </c>
@@ -1822,6 +2031,9 @@
       <c r="A77" t="s">
         <v>78</v>
       </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
       <c r="C77">
         <v>0</v>
       </c>
@@ -1830,6 +2042,9 @@
       <c r="A78" t="s">
         <v>79</v>
       </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
       <c r="C78">
         <v>0</v>
       </c>
@@ -1838,6 +2053,9 @@
       <c r="A79" t="s">
         <v>80</v>
       </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
       <c r="C79">
         <v>0</v>
       </c>
@@ -1846,6 +2064,9 @@
       <c r="A80" t="s">
         <v>81</v>
       </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
       <c r="C80">
         <v>0</v>
       </c>
@@ -1854,6 +2075,9 @@
       <c r="A81" t="s">
         <v>82</v>
       </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
       <c r="C81">
         <v>0</v>
       </c>
@@ -1863,16 +2087,19 @@
         <v>83</v>
       </c>
       <c r="B82">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>59.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>84</v>
       </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
       <c r="C83">
         <v>0</v>
       </c>
@@ -1881,6 +2108,9 @@
       <c r="A84" t="s">
         <v>85</v>
       </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
       <c r="C84">
         <v>0</v>
       </c>
@@ -1889,6 +2119,9 @@
       <c r="A85" t="s">
         <v>86</v>
       </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
       <c r="C85">
         <v>0</v>
       </c>
@@ -1897,6 +2130,9 @@
       <c r="A86" t="s">
         <v>87</v>
       </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
       <c r="C86">
         <v>0</v>
       </c>
@@ -1905,6 +2141,9 @@
       <c r="A87" t="s">
         <v>88</v>
       </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
       <c r="C87">
         <v>0</v>
       </c>
@@ -1913,6 +2152,9 @@
       <c r="A88" t="s">
         <v>89</v>
       </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
       <c r="C88">
         <v>0</v>
       </c>
@@ -1921,6 +2163,9 @@
       <c r="A89" t="s">
         <v>90</v>
       </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
       <c r="C89">
         <v>0</v>
       </c>
@@ -1929,6 +2174,9 @@
       <c r="A90" t="s">
         <v>91</v>
       </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
       <c r="C90">
         <v>0</v>
       </c>
@@ -1937,6 +2185,9 @@
       <c r="A91" t="s">
         <v>92</v>
       </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
       <c r="C91">
         <v>0</v>
       </c>
@@ -1945,6 +2196,9 @@
       <c r="A92" t="s">
         <v>93</v>
       </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
       <c r="C92">
         <v>0</v>
       </c>
@@ -1953,6 +2207,9 @@
       <c r="A93" t="s">
         <v>94</v>
       </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
       <c r="C93">
         <v>0</v>
       </c>
@@ -1961,6 +2218,9 @@
       <c r="A94" t="s">
         <v>95</v>
       </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
       <c r="C94">
         <v>0</v>
       </c>
@@ -1969,6 +2229,9 @@
       <c r="A95" t="s">
         <v>96</v>
       </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
       <c r="C95">
         <v>0</v>
       </c>
@@ -1977,6 +2240,9 @@
       <c r="A96" t="s">
         <v>97</v>
       </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
       <c r="C96">
         <v>0</v>
       </c>
@@ -1985,6 +2251,9 @@
       <c r="A97" t="s">
         <v>98</v>
       </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
       <c r="C97">
         <v>0</v>
       </c>
@@ -1993,6 +2262,9 @@
       <c r="A98" t="s">
         <v>99</v>
       </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
       <c r="C98">
         <v>0</v>
       </c>
@@ -2000,6 +2272,9 @@
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>100</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
       </c>
       <c r="C99">
         <v>0</v>

</xml_diff>